<commit_message>
generate section monthly attendance
</commit_message>
<xml_diff>
--- a/assets/templates/student-attendance-template.xlsx
+++ b/assets/templates/student-attendance-template.xlsx
@@ -194,7 +194,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,7 +204,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE8E8E9"/>
-        <bgColor rgb="FFE8F2D3"/>
+        <bgColor rgb="FFE7DEC9"/>
       </patternFill>
     </fill>
     <fill>
@@ -215,20 +215,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6B07E"/>
-        <bgColor rgb="FFA6A6A6"/>
+        <fgColor rgb="FF00AAAD"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE8F2D3"/>
-        <bgColor rgb="FFE8E8E9"/>
+        <fgColor rgb="FFE9AF90"/>
+        <bgColor rgb="FFF5D28B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBEE3D3"/>
+        <bgColor rgb="FFE7DEC9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF1CE"/>
-        <bgColor rgb="FFE8F2D3"/>
+        <bgColor rgb="FFE8E8E9"/>
       </patternFill>
     </fill>
   </fills>
@@ -343,7 +349,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -408,23 +414,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -442,6 +452,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -469,8 +483,8 @@
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC6B07E"/>
+      <rgbColor rgb="FF00AAAD"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -490,10 +504,10 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFE8F2D3"/>
+      <rgbColor rgb="FFBEE3D3"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFE9AF90"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFF5D28B"/>
       <rgbColor rgb="FF3366FF"/>
@@ -525,8 +539,8 @@
   </sheetPr>
   <dimension ref="B1:AMJ30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AM8" activeCellId="0" sqref="AM8"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y12" activeCellId="0" sqref="Y11:Z12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -755,1871 +769,1871 @@
       <c r="AH5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="AI5" s="14" t="s">
+      <c r="AI5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="AJ5" s="14" t="s">
+      <c r="AJ5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="AK5" s="14" t="s">
+      <c r="AK5" s="17" t="s">
         <v>13</v>
       </c>
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="18" t="n">
+      <c r="C6" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="18" t="n">
+      <c r="D6" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E6" s="18" t="n">
+      <c r="E6" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="18" t="n">
+      <c r="F6" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="G6" s="18" t="n">
+      <c r="G6" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="H6" s="18" t="n">
+      <c r="H6" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="I6" s="18" t="n">
+      <c r="I6" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="J6" s="18" t="n">
+      <c r="J6" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="K6" s="18" t="n">
+      <c r="K6" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="L6" s="18" t="n">
+      <c r="L6" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="M6" s="18" t="n">
+      <c r="M6" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="N6" s="18" t="n">
+      <c r="N6" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="O6" s="18" t="n">
+      <c r="O6" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="P6" s="18" t="n">
+      <c r="P6" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="Q6" s="18" t="n">
+      <c r="Q6" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="R6" s="18" t="n">
+      <c r="R6" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="S6" s="18" t="n">
+      <c r="S6" s="19" t="n">
         <v>17</v>
       </c>
-      <c r="T6" s="18" t="n">
+      <c r="T6" s="19" t="n">
         <v>18</v>
       </c>
-      <c r="U6" s="18" t="n">
+      <c r="U6" s="19" t="n">
         <v>19</v>
       </c>
-      <c r="V6" s="18" t="n">
+      <c r="V6" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="W6" s="18" t="n">
+      <c r="W6" s="19" t="n">
         <v>21</v>
       </c>
-      <c r="X6" s="18" t="n">
+      <c r="X6" s="19" t="n">
         <v>22</v>
       </c>
-      <c r="Y6" s="18" t="n">
+      <c r="Y6" s="19" t="n">
         <v>23</v>
       </c>
-      <c r="Z6" s="18" t="n">
+      <c r="Z6" s="19" t="n">
         <v>24</v>
       </c>
-      <c r="AA6" s="18" t="n">
+      <c r="AA6" s="19" t="n">
         <v>25</v>
       </c>
-      <c r="AB6" s="18" t="n">
+      <c r="AB6" s="19" t="n">
         <v>26</v>
       </c>
-      <c r="AC6" s="18" t="n">
+      <c r="AC6" s="19" t="n">
         <v>27</v>
       </c>
-      <c r="AD6" s="18" t="n">
+      <c r="AD6" s="19" t="n">
         <v>28</v>
       </c>
-      <c r="AE6" s="18" t="n">
+      <c r="AE6" s="19" t="n">
         <v>29</v>
       </c>
-      <c r="AF6" s="18" t="n">
+      <c r="AF6" s="19" t="n">
         <v>30</v>
       </c>
-      <c r="AG6" s="18" t="n">
+      <c r="AG6" s="19" t="n">
         <v>31</v>
       </c>
-      <c r="AH6" s="19" t="n">
+      <c r="AH6" s="20" t="n">
         <f aca="false">COUNTIF($C7:$AG7,"T")</f>
         <v>0</v>
       </c>
-      <c r="AI6" s="20" t="n">
+      <c r="AI6" s="21" t="n">
         <f aca="false">COUNTIF($C7:$AG7,"U")</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="20" t="n">
+      <c r="AJ6" s="21" t="n">
         <f aca="false">COUNTIF($C7:$AG7,"E")</f>
         <v>0</v>
       </c>
-      <c r="AK6" s="20" t="n">
+      <c r="AK6" s="21" t="n">
         <f aca="false">COUNTIF($C7:$AG7,"P")</f>
         <v>0</v>
       </c>
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="17"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
       <c r="W7" s="10"/>
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
       <c r="AA7" s="10"/>
-      <c r="AB7" s="21"/>
-      <c r="AC7" s="21"/>
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="22"/>
       <c r="AD7" s="10"/>
       <c r="AE7" s="10"/>
       <c r="AF7" s="10"/>
       <c r="AG7" s="10"/>
-      <c r="AH7" s="19"/>
-      <c r="AI7" s="20"/>
-      <c r="AJ7" s="20"/>
-      <c r="AK7" s="20"/>
+      <c r="AH7" s="20"/>
+      <c r="AI7" s="21"/>
+      <c r="AJ7" s="21"/>
+      <c r="AK7" s="21"/>
       <c r="AMJ7" s="0"/>
     </row>
     <row r="8" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="18" t="n">
+      <c r="C8" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="18" t="n">
+      <c r="D8" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E8" s="18" t="n">
+      <c r="E8" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F8" s="18" t="n">
+      <c r="F8" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="G8" s="18" t="n">
+      <c r="G8" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="H8" s="18" t="n">
+      <c r="H8" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="I8" s="18" t="n">
+      <c r="I8" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="J8" s="18" t="n">
+      <c r="J8" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="K8" s="18" t="n">
+      <c r="K8" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="L8" s="18" t="n">
+      <c r="L8" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="M8" s="18" t="n">
+      <c r="M8" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="N8" s="18" t="n">
+      <c r="N8" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="O8" s="18" t="n">
+      <c r="O8" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="P8" s="18" t="n">
+      <c r="P8" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="Q8" s="18" t="n">
+      <c r="Q8" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="R8" s="18" t="n">
+      <c r="R8" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="S8" s="18" t="n">
+      <c r="S8" s="19" t="n">
         <v>17</v>
       </c>
-      <c r="T8" s="18" t="n">
+      <c r="T8" s="19" t="n">
         <v>18</v>
       </c>
-      <c r="U8" s="18" t="n">
+      <c r="U8" s="19" t="n">
         <v>19</v>
       </c>
-      <c r="V8" s="18" t="n">
+      <c r="V8" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="W8" s="18" t="n">
+      <c r="W8" s="19" t="n">
         <v>21</v>
       </c>
-      <c r="X8" s="18" t="n">
+      <c r="X8" s="19" t="n">
         <v>22</v>
       </c>
-      <c r="Y8" s="18" t="n">
+      <c r="Y8" s="19" t="n">
         <v>23</v>
       </c>
-      <c r="Z8" s="18" t="n">
+      <c r="Z8" s="19" t="n">
         <v>24</v>
       </c>
-      <c r="AA8" s="18" t="n">
+      <c r="AA8" s="19" t="n">
         <v>25</v>
       </c>
-      <c r="AB8" s="18" t="n">
+      <c r="AB8" s="19" t="n">
         <v>26</v>
       </c>
-      <c r="AC8" s="18" t="n">
+      <c r="AC8" s="19" t="n">
         <v>27</v>
       </c>
-      <c r="AD8" s="18" t="n">
+      <c r="AD8" s="19" t="n">
         <v>28</v>
       </c>
-      <c r="AE8" s="18" t="n">
+      <c r="AE8" s="19" t="n">
         <v>29</v>
       </c>
-      <c r="AF8" s="18" t="n">
+      <c r="AF8" s="19" t="n">
         <v>30</v>
       </c>
-      <c r="AG8" s="18"/>
-      <c r="AH8" s="19" t="n">
+      <c r="AG8" s="19"/>
+      <c r="AH8" s="20" t="n">
         <f aca="false">COUNTIF($C9:$AF9,"T")</f>
         <v>0</v>
       </c>
-      <c r="AI8" s="20" t="n">
+      <c r="AI8" s="21" t="n">
         <f aca="false">COUNTIF($C9:$AF9,"U")</f>
         <v>0</v>
       </c>
-      <c r="AJ8" s="20" t="n">
+      <c r="AJ8" s="21" t="n">
         <f aca="false">COUNTIF($C9:$AF9,"E")</f>
         <v>0</v>
       </c>
-      <c r="AK8" s="20" t="n">
+      <c r="AK8" s="21" t="n">
         <f aca="false">COUNTIF($C9:$AF9,"P")</f>
         <v>0</v>
       </c>
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="17"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="10"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
       <c r="X9" s="10"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
       <c r="AA9" s="10"/>
       <c r="AB9" s="10"/>
       <c r="AC9" s="10"/>
       <c r="AD9" s="10"/>
       <c r="AE9" s="10"/>
-      <c r="AF9" s="21"/>
-      <c r="AG9" s="22"/>
-      <c r="AH9" s="19"/>
-      <c r="AI9" s="20"/>
-      <c r="AJ9" s="20"/>
-      <c r="AK9" s="20"/>
-      <c r="AL9" s="23"/>
+      <c r="AF9" s="22"/>
+      <c r="AG9" s="23"/>
+      <c r="AH9" s="20"/>
+      <c r="AI9" s="21"/>
+      <c r="AJ9" s="21"/>
+      <c r="AK9" s="21"/>
+      <c r="AL9" s="24"/>
       <c r="AMJ9" s="0"/>
     </row>
     <row r="10" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="18" t="n">
+      <c r="C10" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="18" t="n">
+      <c r="D10" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E10" s="18" t="n">
+      <c r="E10" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F10" s="18" t="n">
+      <c r="F10" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="G10" s="18" t="n">
+      <c r="G10" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="H10" s="18" t="n">
+      <c r="H10" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="I10" s="18" t="n">
+      <c r="I10" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="J10" s="18" t="n">
+      <c r="J10" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="K10" s="18" t="n">
+      <c r="K10" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="L10" s="18" t="n">
+      <c r="L10" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="M10" s="18" t="n">
+      <c r="M10" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="N10" s="18" t="n">
+      <c r="N10" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="O10" s="18" t="n">
+      <c r="O10" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="P10" s="18" t="n">
+      <c r="P10" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="Q10" s="18" t="n">
+      <c r="Q10" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="R10" s="18" t="n">
+      <c r="R10" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="S10" s="18" t="n">
+      <c r="S10" s="19" t="n">
         <v>17</v>
       </c>
-      <c r="T10" s="18" t="n">
+      <c r="T10" s="19" t="n">
         <v>18</v>
       </c>
-      <c r="U10" s="18" t="n">
+      <c r="U10" s="19" t="n">
         <v>19</v>
       </c>
-      <c r="V10" s="18" t="n">
+      <c r="V10" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="W10" s="18" t="n">
+      <c r="W10" s="19" t="n">
         <v>21</v>
       </c>
-      <c r="X10" s="18" t="n">
+      <c r="X10" s="19" t="n">
         <v>22</v>
       </c>
-      <c r="Y10" s="18" t="n">
+      <c r="Y10" s="19" t="n">
         <v>23</v>
       </c>
-      <c r="Z10" s="18" t="n">
+      <c r="Z10" s="19" t="n">
         <v>24</v>
       </c>
-      <c r="AA10" s="18" t="n">
+      <c r="AA10" s="19" t="n">
         <v>25</v>
       </c>
-      <c r="AB10" s="18" t="n">
+      <c r="AB10" s="19" t="n">
         <v>26</v>
       </c>
-      <c r="AC10" s="18" t="n">
+      <c r="AC10" s="19" t="n">
         <v>27</v>
       </c>
-      <c r="AD10" s="18" t="n">
+      <c r="AD10" s="19" t="n">
         <v>28</v>
       </c>
-      <c r="AE10" s="18" t="n">
+      <c r="AE10" s="19" t="n">
         <v>29</v>
       </c>
-      <c r="AF10" s="18" t="n">
+      <c r="AF10" s="19" t="n">
         <v>30</v>
       </c>
-      <c r="AG10" s="18" t="n">
+      <c r="AG10" s="19" t="n">
         <v>31</v>
       </c>
-      <c r="AH10" s="19" t="n">
+      <c r="AH10" s="20" t="n">
         <f aca="false">COUNTIF($C11:$AG11,"T")</f>
         <v>0</v>
       </c>
-      <c r="AI10" s="20" t="n">
+      <c r="AI10" s="21" t="n">
         <f aca="false">COUNTIF($C11:$AG11,"U")</f>
         <v>0</v>
       </c>
-      <c r="AJ10" s="20" t="n">
+      <c r="AJ10" s="21" t="n">
         <f aca="false">COUNTIF($C11:$AG11,"E")</f>
         <v>0</v>
       </c>
-      <c r="AK10" s="20" t="n">
+      <c r="AK10" s="21" t="n">
         <f aca="false">COUNTIF($C11:$AG11,"P")</f>
         <v>0</v>
       </c>
       <c r="AMJ10" s="0"/>
     </row>
     <row r="11" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="17"/>
-      <c r="C11" s="21"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="21"/>
+      <c r="W11" s="22"/>
+      <c r="X11" s="22"/>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
       <c r="AA11" s="10"/>
       <c r="AB11" s="10"/>
       <c r="AC11" s="10"/>
-      <c r="AD11" s="21"/>
-      <c r="AE11" s="21"/>
+      <c r="AD11" s="22"/>
+      <c r="AE11" s="22"/>
       <c r="AF11" s="10"/>
       <c r="AG11" s="10"/>
-      <c r="AH11" s="19"/>
-      <c r="AI11" s="20"/>
-      <c r="AJ11" s="20"/>
-      <c r="AK11" s="20"/>
+      <c r="AH11" s="20"/>
+      <c r="AI11" s="21"/>
+      <c r="AJ11" s="21"/>
+      <c r="AK11" s="21"/>
       <c r="AMJ11" s="0"/>
     </row>
     <row r="12" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="18" t="n">
+      <c r="C12" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D12" s="18" t="n">
+      <c r="D12" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E12" s="18" t="n">
+      <c r="E12" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F12" s="18" t="n">
+      <c r="F12" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="G12" s="18" t="n">
+      <c r="G12" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="H12" s="18" t="n">
+      <c r="H12" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="I12" s="18" t="n">
+      <c r="I12" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="J12" s="18" t="n">
+      <c r="J12" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="K12" s="18" t="n">
+      <c r="K12" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="L12" s="18" t="n">
+      <c r="L12" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="M12" s="18" t="n">
+      <c r="M12" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="N12" s="18" t="n">
+      <c r="N12" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="O12" s="18" t="n">
+      <c r="O12" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="P12" s="18" t="n">
+      <c r="P12" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="Q12" s="18" t="n">
+      <c r="Q12" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="R12" s="18" t="n">
+      <c r="R12" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="S12" s="18" t="n">
+      <c r="S12" s="19" t="n">
         <v>17</v>
       </c>
-      <c r="T12" s="18" t="n">
+      <c r="T12" s="19" t="n">
         <v>18</v>
       </c>
-      <c r="U12" s="18" t="n">
+      <c r="U12" s="19" t="n">
         <v>19</v>
       </c>
-      <c r="V12" s="18" t="n">
+      <c r="V12" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="W12" s="18" t="n">
+      <c r="W12" s="19" t="n">
         <v>21</v>
       </c>
-      <c r="X12" s="18" t="n">
+      <c r="X12" s="19" t="n">
         <v>22</v>
       </c>
-      <c r="Y12" s="18" t="n">
+      <c r="Y12" s="19" t="n">
         <v>23</v>
       </c>
-      <c r="Z12" s="18" t="n">
+      <c r="Z12" s="19" t="n">
         <v>24</v>
       </c>
-      <c r="AA12" s="18" t="n">
+      <c r="AA12" s="19" t="n">
         <v>25</v>
       </c>
-      <c r="AB12" s="18" t="n">
+      <c r="AB12" s="19" t="n">
         <v>26</v>
       </c>
-      <c r="AC12" s="18" t="n">
+      <c r="AC12" s="19" t="n">
         <v>27</v>
       </c>
-      <c r="AD12" s="18" t="n">
+      <c r="AD12" s="19" t="n">
         <v>28</v>
       </c>
-      <c r="AE12" s="18" t="n">
+      <c r="AE12" s="19" t="n">
         <v>29</v>
       </c>
-      <c r="AF12" s="18" t="n">
+      <c r="AF12" s="19" t="n">
         <v>30</v>
       </c>
-      <c r="AG12" s="18"/>
-      <c r="AH12" s="19" t="n">
+      <c r="AG12" s="19"/>
+      <c r="AH12" s="20" t="n">
         <f aca="false">COUNTIF($C13:$AF13,"T")</f>
         <v>0</v>
       </c>
-      <c r="AI12" s="20" t="n">
+      <c r="AI12" s="21" t="n">
         <f aca="false">COUNTIF($C13:$AF13,"U")</f>
         <v>0</v>
       </c>
-      <c r="AJ12" s="20" t="n">
+      <c r="AJ12" s="21" t="n">
         <f aca="false">COUNTIF($C13:$AF13,"E")</f>
         <v>0</v>
       </c>
-      <c r="AK12" s="20" t="n">
+      <c r="AK12" s="21" t="n">
         <f aca="false">COUNTIF($C13:$AF13,"P")</f>
         <v>0</v>
       </c>
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="17"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
+      <c r="T13" s="22"/>
+      <c r="U13" s="22"/>
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
-      <c r="AA13" s="21"/>
-      <c r="AB13" s="21"/>
+      <c r="AA13" s="22"/>
+      <c r="AB13" s="22"/>
       <c r="AC13" s="10"/>
       <c r="AD13" s="10"/>
       <c r="AE13" s="10"/>
       <c r="AF13" s="10"/>
-      <c r="AG13" s="22"/>
-      <c r="AH13" s="19"/>
-      <c r="AI13" s="20"/>
-      <c r="AJ13" s="20"/>
-      <c r="AK13" s="20"/>
+      <c r="AG13" s="23"/>
+      <c r="AH13" s="20"/>
+      <c r="AI13" s="21"/>
+      <c r="AJ13" s="21"/>
+      <c r="AK13" s="21"/>
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="18" t="n">
+      <c r="C14" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D14" s="18" t="n">
+      <c r="D14" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E14" s="18" t="n">
+      <c r="E14" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F14" s="18" t="n">
+      <c r="F14" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="G14" s="18" t="n">
+      <c r="G14" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="H14" s="18" t="n">
+      <c r="H14" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="I14" s="18" t="n">
+      <c r="I14" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="J14" s="18" t="n">
+      <c r="J14" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="K14" s="18" t="n">
+      <c r="K14" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="L14" s="18" t="n">
+      <c r="L14" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="M14" s="18" t="n">
+      <c r="M14" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="N14" s="18" t="n">
+      <c r="N14" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="O14" s="18" t="n">
+      <c r="O14" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="P14" s="18" t="n">
+      <c r="P14" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="Q14" s="18" t="n">
+      <c r="Q14" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="R14" s="18" t="n">
+      <c r="R14" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="S14" s="18" t="n">
+      <c r="S14" s="19" t="n">
         <v>17</v>
       </c>
-      <c r="T14" s="18" t="n">
+      <c r="T14" s="19" t="n">
         <v>18</v>
       </c>
-      <c r="U14" s="18" t="n">
+      <c r="U14" s="19" t="n">
         <v>19</v>
       </c>
-      <c r="V14" s="18" t="n">
+      <c r="V14" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="W14" s="18" t="n">
+      <c r="W14" s="19" t="n">
         <v>21</v>
       </c>
-      <c r="X14" s="18" t="n">
+      <c r="X14" s="19" t="n">
         <v>22</v>
       </c>
-      <c r="Y14" s="18" t="n">
+      <c r="Y14" s="19" t="n">
         <v>23</v>
       </c>
-      <c r="Z14" s="18" t="n">
+      <c r="Z14" s="19" t="n">
         <v>24</v>
       </c>
-      <c r="AA14" s="18" t="n">
+      <c r="AA14" s="19" t="n">
         <v>25</v>
       </c>
-      <c r="AB14" s="18" t="n">
+      <c r="AB14" s="19" t="n">
         <v>26</v>
       </c>
-      <c r="AC14" s="18" t="n">
+      <c r="AC14" s="19" t="n">
         <v>27</v>
       </c>
-      <c r="AD14" s="18" t="n">
+      <c r="AD14" s="19" t="n">
         <v>28</v>
       </c>
-      <c r="AE14" s="18" t="n">
+      <c r="AE14" s="19" t="n">
         <v>29</v>
       </c>
-      <c r="AF14" s="18" t="n">
+      <c r="AF14" s="19" t="n">
         <v>30</v>
       </c>
-      <c r="AG14" s="18" t="n">
+      <c r="AG14" s="19" t="n">
         <v>31</v>
       </c>
-      <c r="AH14" s="19" t="n">
+      <c r="AH14" s="20" t="n">
         <f aca="false">COUNTIF($C15:$AG15,"T")</f>
         <v>0</v>
       </c>
-      <c r="AI14" s="20" t="n">
+      <c r="AI14" s="21" t="n">
         <f aca="false">COUNTIF($C15:$AG15,"U")</f>
         <v>0</v>
       </c>
-      <c r="AJ14" s="20" t="n">
+      <c r="AJ14" s="21" t="n">
         <f aca="false">COUNTIF($C15:$AG15,"E")</f>
         <v>0</v>
       </c>
-      <c r="AK14" s="20" t="n">
+      <c r="AK14" s="21" t="n">
         <f aca="false">COUNTIF($C15:$AG15,"P")</f>
         <v>0</v>
       </c>
       <c r="AMJ14" s="0"/>
     </row>
     <row r="15" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="17"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="10"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
       <c r="T15" s="10"/>
       <c r="U15" s="10"/>
       <c r="V15" s="10"/>
       <c r="W15" s="10"/>
       <c r="X15" s="10"/>
-      <c r="Y15" s="21"/>
-      <c r="Z15" s="21"/>
+      <c r="Y15" s="22"/>
+      <c r="Z15" s="22"/>
       <c r="AA15" s="10"/>
       <c r="AB15" s="10"/>
       <c r="AC15" s="10"/>
       <c r="AD15" s="10"/>
       <c r="AE15" s="10"/>
-      <c r="AF15" s="21"/>
-      <c r="AG15" s="21"/>
-      <c r="AH15" s="19"/>
-      <c r="AI15" s="20"/>
-      <c r="AJ15" s="20"/>
-      <c r="AK15" s="20"/>
+      <c r="AF15" s="22"/>
+      <c r="AG15" s="22"/>
+      <c r="AH15" s="20"/>
+      <c r="AI15" s="21"/>
+      <c r="AJ15" s="21"/>
+      <c r="AK15" s="21"/>
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="18" t="n">
+      <c r="C16" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="18" t="n">
+      <c r="D16" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E16" s="18" t="n">
+      <c r="E16" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F16" s="18" t="n">
+      <c r="F16" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="G16" s="18" t="n">
+      <c r="G16" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="H16" s="18" t="n">
+      <c r="H16" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="I16" s="18" t="n">
+      <c r="I16" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="J16" s="18" t="n">
+      <c r="J16" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="K16" s="18" t="n">
+      <c r="K16" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="L16" s="18" t="n">
+      <c r="L16" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="M16" s="18" t="n">
+      <c r="M16" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="N16" s="18" t="n">
+      <c r="N16" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="O16" s="18" t="n">
+      <c r="O16" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="P16" s="18" t="n">
+      <c r="P16" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="Q16" s="18" t="n">
+      <c r="Q16" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="R16" s="18" t="n">
+      <c r="R16" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="S16" s="18" t="n">
+      <c r="S16" s="19" t="n">
         <v>17</v>
       </c>
-      <c r="T16" s="18" t="n">
+      <c r="T16" s="19" t="n">
         <v>18</v>
       </c>
-      <c r="U16" s="18" t="n">
+      <c r="U16" s="19" t="n">
         <v>19</v>
       </c>
-      <c r="V16" s="18" t="n">
+      <c r="V16" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="W16" s="18" t="n">
+      <c r="W16" s="19" t="n">
         <v>21</v>
       </c>
-      <c r="X16" s="18" t="n">
+      <c r="X16" s="19" t="n">
         <v>22</v>
       </c>
-      <c r="Y16" s="18" t="n">
+      <c r="Y16" s="19" t="n">
         <v>23</v>
       </c>
-      <c r="Z16" s="18" t="n">
+      <c r="Z16" s="19" t="n">
         <v>24</v>
       </c>
-      <c r="AA16" s="18" t="n">
+      <c r="AA16" s="19" t="n">
         <v>25</v>
       </c>
-      <c r="AB16" s="18" t="n">
+      <c r="AB16" s="19" t="n">
         <v>26</v>
       </c>
-      <c r="AC16" s="18" t="n">
+      <c r="AC16" s="19" t="n">
         <v>27</v>
       </c>
-      <c r="AD16" s="18" t="n">
+      <c r="AD16" s="19" t="n">
         <v>28</v>
       </c>
-      <c r="AE16" s="18" t="n">
+      <c r="AE16" s="19" t="n">
         <v>29</v>
       </c>
-      <c r="AF16" s="18" t="n">
+      <c r="AF16" s="19" t="n">
         <v>30</v>
       </c>
-      <c r="AG16" s="18" t="n">
+      <c r="AG16" s="19" t="n">
         <v>31</v>
       </c>
-      <c r="AH16" s="19" t="n">
+      <c r="AH16" s="20" t="n">
         <f aca="false">COUNTIF($C17:$AG17,"T")</f>
         <v>0</v>
       </c>
-      <c r="AI16" s="20" t="n">
+      <c r="AI16" s="21" t="n">
         <f aca="false">COUNTIF($C17:$AG17,"U")</f>
         <v>0</v>
       </c>
-      <c r="AJ16" s="20" t="n">
+      <c r="AJ16" s="21" t="n">
         <f aca="false">COUNTIF($C17:$AG17,"E")</f>
         <v>0</v>
       </c>
-      <c r="AK16" s="20" t="n">
+      <c r="AK16" s="21" t="n">
         <f aca="false">COUNTIF($C17:$AG17,"P")</f>
         <v>0</v>
       </c>
       <c r="AMJ16" s="0"/>
     </row>
     <row r="17" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="17"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
       <c r="U17" s="10"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="21"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
       <c r="X17" s="10"/>
       <c r="Y17" s="10"/>
       <c r="Z17" s="10"/>
       <c r="AA17" s="10"/>
       <c r="AB17" s="10"/>
-      <c r="AC17" s="21"/>
-      <c r="AD17" s="21"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22"/>
       <c r="AE17" s="10"/>
       <c r="AF17" s="10"/>
       <c r="AG17" s="10"/>
-      <c r="AH17" s="19"/>
-      <c r="AI17" s="20"/>
-      <c r="AJ17" s="20"/>
-      <c r="AK17" s="20"/>
+      <c r="AH17" s="20"/>
+      <c r="AI17" s="21"/>
+      <c r="AJ17" s="21"/>
+      <c r="AK17" s="21"/>
       <c r="AMJ17" s="0"/>
     </row>
     <row r="18" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="18" t="n">
+      <c r="C18" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D18" s="18" t="n">
+      <c r="D18" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E18" s="18" t="n">
+      <c r="E18" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F18" s="18" t="n">
+      <c r="F18" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="G18" s="18" t="n">
+      <c r="G18" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="H18" s="18" t="n">
+      <c r="H18" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="I18" s="18" t="n">
+      <c r="I18" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="J18" s="18" t="n">
+      <c r="J18" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="K18" s="18" t="n">
+      <c r="K18" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="L18" s="18" t="n">
+      <c r="L18" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="M18" s="18" t="n">
+      <c r="M18" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="N18" s="18" t="n">
+      <c r="N18" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="O18" s="18" t="n">
+      <c r="O18" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="P18" s="18" t="n">
+      <c r="P18" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="Q18" s="18" t="n">
+      <c r="Q18" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="R18" s="18" t="n">
+      <c r="R18" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="S18" s="18" t="n">
+      <c r="S18" s="19" t="n">
         <v>17</v>
       </c>
-      <c r="T18" s="18" t="n">
+      <c r="T18" s="19" t="n">
         <v>18</v>
       </c>
-      <c r="U18" s="18" t="n">
+      <c r="U18" s="19" t="n">
         <v>19</v>
       </c>
-      <c r="V18" s="18" t="n">
+      <c r="V18" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="W18" s="18" t="n">
+      <c r="W18" s="19" t="n">
         <v>21</v>
       </c>
-      <c r="X18" s="18" t="n">
+      <c r="X18" s="19" t="n">
         <v>22</v>
       </c>
-      <c r="Y18" s="18" t="n">
+      <c r="Y18" s="19" t="n">
         <v>23</v>
       </c>
-      <c r="Z18" s="18" t="n">
+      <c r="Z18" s="19" t="n">
         <v>24</v>
       </c>
-      <c r="AA18" s="18" t="n">
+      <c r="AA18" s="19" t="n">
         <v>25</v>
       </c>
-      <c r="AB18" s="18" t="n">
+      <c r="AB18" s="19" t="n">
         <v>26</v>
       </c>
-      <c r="AC18" s="18" t="n">
+      <c r="AC18" s="19" t="n">
         <v>27</v>
       </c>
-      <c r="AD18" s="18" t="n">
+      <c r="AD18" s="19" t="n">
         <v>28</v>
       </c>
-      <c r="AE18" s="18"/>
-      <c r="AF18" s="18"/>
-      <c r="AG18" s="18"/>
-      <c r="AH18" s="19" t="n">
+      <c r="AE18" s="19"/>
+      <c r="AF18" s="19"/>
+      <c r="AG18" s="19"/>
+      <c r="AH18" s="20" t="n">
         <f aca="false">COUNTIF($C19:$AD19,"T")</f>
         <v>0</v>
       </c>
-      <c r="AI18" s="20" t="n">
+      <c r="AI18" s="21" t="n">
         <f aca="false">COUNTIF($C19:$AD19,"U")</f>
         <v>0</v>
       </c>
-      <c r="AJ18" s="20" t="n">
+      <c r="AJ18" s="21" t="n">
         <f aca="false">COUNTIF($C19:$AD19,"E")</f>
         <v>0</v>
       </c>
-      <c r="AK18" s="20" t="n">
+      <c r="AK18" s="21" t="n">
         <f aca="false">COUNTIF($C19:$AD19,"P")</f>
         <v>0</v>
       </c>
       <c r="AMJ18" s="0"/>
     </row>
     <row r="19" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="17"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22"/>
       <c r="U19" s="10"/>
       <c r="V19" s="10"/>
       <c r="W19" s="10"/>
       <c r="X19" s="10"/>
       <c r="Y19" s="10"/>
-      <c r="Z19" s="21"/>
-      <c r="AA19" s="21"/>
+      <c r="Z19" s="22"/>
+      <c r="AA19" s="22"/>
       <c r="AB19" s="10"/>
       <c r="AC19" s="10"/>
       <c r="AD19" s="10"/>
-      <c r="AE19" s="22"/>
-      <c r="AF19" s="22"/>
-      <c r="AG19" s="22"/>
-      <c r="AH19" s="19"/>
-      <c r="AI19" s="20"/>
-      <c r="AJ19" s="20"/>
-      <c r="AK19" s="20"/>
+      <c r="AE19" s="23"/>
+      <c r="AF19" s="23"/>
+      <c r="AG19" s="23"/>
+      <c r="AH19" s="20"/>
+      <c r="AI19" s="21"/>
+      <c r="AJ19" s="21"/>
+      <c r="AK19" s="21"/>
       <c r="AMJ19" s="0"/>
     </row>
     <row r="20" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="18" t="n">
+      <c r="C20" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="18" t="n">
+      <c r="D20" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E20" s="18" t="n">
+      <c r="E20" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F20" s="18" t="n">
+      <c r="F20" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="G20" s="18" t="n">
+      <c r="G20" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="H20" s="18" t="n">
+      <c r="H20" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="I20" s="18" t="n">
+      <c r="I20" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="J20" s="18" t="n">
+      <c r="J20" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="K20" s="18" t="n">
+      <c r="K20" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="L20" s="18" t="n">
+      <c r="L20" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="M20" s="18" t="n">
+      <c r="M20" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="N20" s="18" t="n">
+      <c r="N20" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="O20" s="18" t="n">
+      <c r="O20" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="P20" s="18" t="n">
+      <c r="P20" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="Q20" s="18" t="n">
+      <c r="Q20" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="R20" s="18" t="n">
+      <c r="R20" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="S20" s="18" t="n">
+      <c r="S20" s="19" t="n">
         <v>17</v>
       </c>
-      <c r="T20" s="18" t="n">
+      <c r="T20" s="19" t="n">
         <v>18</v>
       </c>
-      <c r="U20" s="18" t="n">
+      <c r="U20" s="19" t="n">
         <v>19</v>
       </c>
-      <c r="V20" s="18" t="n">
+      <c r="V20" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="W20" s="18" t="n">
+      <c r="W20" s="19" t="n">
         <v>21</v>
       </c>
-      <c r="X20" s="18" t="n">
+      <c r="X20" s="19" t="n">
         <v>22</v>
       </c>
-      <c r="Y20" s="18" t="n">
+      <c r="Y20" s="19" t="n">
         <v>23</v>
       </c>
-      <c r="Z20" s="18" t="n">
+      <c r="Z20" s="19" t="n">
         <v>24</v>
       </c>
-      <c r="AA20" s="18" t="n">
+      <c r="AA20" s="19" t="n">
         <v>25</v>
       </c>
-      <c r="AB20" s="18" t="n">
+      <c r="AB20" s="19" t="n">
         <v>26</v>
       </c>
-      <c r="AC20" s="18" t="n">
+      <c r="AC20" s="19" t="n">
         <v>27</v>
       </c>
-      <c r="AD20" s="18" t="n">
+      <c r="AD20" s="19" t="n">
         <v>28</v>
       </c>
-      <c r="AE20" s="18" t="n">
+      <c r="AE20" s="19" t="n">
         <v>29</v>
       </c>
-      <c r="AF20" s="18" t="n">
+      <c r="AF20" s="19" t="n">
         <v>30</v>
       </c>
-      <c r="AG20" s="18" t="n">
+      <c r="AG20" s="19" t="n">
         <v>31</v>
       </c>
-      <c r="AH20" s="19" t="n">
+      <c r="AH20" s="20" t="n">
         <f aca="false">COUNTIF($C21:$AG21,"T")</f>
         <v>0</v>
       </c>
-      <c r="AI20" s="20" t="n">
+      <c r="AI20" s="21" t="n">
         <f aca="false">COUNTIF($C21:$AG21,"U")</f>
         <v>0</v>
       </c>
-      <c r="AJ20" s="20" t="n">
+      <c r="AJ20" s="21" t="n">
         <f aca="false">COUNTIF($C21:$AG21,"E")</f>
         <v>0</v>
       </c>
-      <c r="AK20" s="20" t="n">
+      <c r="AK20" s="21" t="n">
         <f aca="false">COUNTIF($C21:$AG21,"P")</f>
         <v>0</v>
       </c>
       <c r="AMJ20" s="0"/>
     </row>
     <row r="21" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="17"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
       <c r="U21" s="10"/>
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
       <c r="X21" s="10"/>
       <c r="Y21" s="10"/>
-      <c r="Z21" s="21"/>
-      <c r="AA21" s="21"/>
+      <c r="Z21" s="22"/>
+      <c r="AA21" s="22"/>
       <c r="AB21" s="10"/>
       <c r="AC21" s="10"/>
       <c r="AD21" s="10"/>
       <c r="AE21" s="10"/>
       <c r="AF21" s="10"/>
-      <c r="AG21" s="21"/>
-      <c r="AH21" s="19"/>
-      <c r="AI21" s="20"/>
-      <c r="AJ21" s="20"/>
-      <c r="AK21" s="20"/>
+      <c r="AG21" s="22"/>
+      <c r="AH21" s="20"/>
+      <c r="AI21" s="21"/>
+      <c r="AJ21" s="21"/>
+      <c r="AK21" s="21"/>
       <c r="AMJ21" s="0"/>
     </row>
     <row r="22" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="18" t="n">
+      <c r="C22" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="18" t="n">
+      <c r="D22" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="18" t="n">
+      <c r="E22" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F22" s="18" t="n">
+      <c r="F22" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="G22" s="18" t="n">
+      <c r="G22" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="H22" s="18" t="n">
+      <c r="H22" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="I22" s="18" t="n">
+      <c r="I22" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="J22" s="18" t="n">
+      <c r="J22" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="K22" s="18" t="n">
+      <c r="K22" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="L22" s="18" t="n">
+      <c r="L22" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="M22" s="18" t="n">
+      <c r="M22" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="N22" s="18" t="n">
+      <c r="N22" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="O22" s="18" t="n">
+      <c r="O22" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="P22" s="18" t="n">
+      <c r="P22" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="Q22" s="18" t="n">
+      <c r="Q22" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="R22" s="18" t="n">
+      <c r="R22" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="S22" s="18" t="n">
+      <c r="S22" s="19" t="n">
         <v>17</v>
       </c>
-      <c r="T22" s="18" t="n">
+      <c r="T22" s="19" t="n">
         <v>18</v>
       </c>
-      <c r="U22" s="18" t="n">
+      <c r="U22" s="19" t="n">
         <v>19</v>
       </c>
-      <c r="V22" s="18" t="n">
+      <c r="V22" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="W22" s="18" t="n">
+      <c r="W22" s="19" t="n">
         <v>21</v>
       </c>
-      <c r="X22" s="18" t="n">
+      <c r="X22" s="19" t="n">
         <v>22</v>
       </c>
-      <c r="Y22" s="18" t="n">
+      <c r="Y22" s="19" t="n">
         <v>23</v>
       </c>
-      <c r="Z22" s="18" t="n">
+      <c r="Z22" s="19" t="n">
         <v>24</v>
       </c>
-      <c r="AA22" s="18" t="n">
+      <c r="AA22" s="19" t="n">
         <v>25</v>
       </c>
-      <c r="AB22" s="18" t="n">
+      <c r="AB22" s="19" t="n">
         <v>26</v>
       </c>
-      <c r="AC22" s="18" t="n">
+      <c r="AC22" s="19" t="n">
         <v>27</v>
       </c>
-      <c r="AD22" s="18" t="n">
+      <c r="AD22" s="19" t="n">
         <v>28</v>
       </c>
-      <c r="AE22" s="18" t="n">
+      <c r="AE22" s="19" t="n">
         <v>29</v>
       </c>
-      <c r="AF22" s="18" t="n">
+      <c r="AF22" s="19" t="n">
         <v>30</v>
       </c>
-      <c r="AG22" s="18"/>
-      <c r="AH22" s="19" t="n">
+      <c r="AG22" s="19"/>
+      <c r="AH22" s="20" t="n">
         <f aca="false">COUNTIF($C23:$AF23,"T")</f>
         <v>0</v>
       </c>
-      <c r="AI22" s="20" t="n">
+      <c r="AI22" s="21" t="n">
         <f aca="false">COUNTIF($C23:$AF23,"U")</f>
         <v>0</v>
       </c>
-      <c r="AJ22" s="20" t="n">
+      <c r="AJ22" s="21" t="n">
         <f aca="false">COUNTIF($C23:$AF23,"E")</f>
         <v>0</v>
       </c>
-      <c r="AK22" s="20" t="n">
+      <c r="AK22" s="21" t="n">
         <f aca="false">COUNTIF($C23:$AF23,"P")</f>
         <v>0</v>
       </c>
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="17"/>
-      <c r="C23" s="21"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="22"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
-      <c r="P23" s="21"/>
-      <c r="Q23" s="21"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
       <c r="T23" s="10"/>
       <c r="U23" s="10"/>
       <c r="V23" s="10"/>
-      <c r="W23" s="21"/>
-      <c r="X23" s="21"/>
+      <c r="W23" s="22"/>
+      <c r="X23" s="22"/>
       <c r="Y23" s="10"/>
       <c r="Z23" s="10"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="10"/>
       <c r="AC23" s="10"/>
-      <c r="AD23" s="21"/>
-      <c r="AE23" s="21"/>
+      <c r="AD23" s="22"/>
+      <c r="AE23" s="22"/>
       <c r="AF23" s="10"/>
-      <c r="AG23" s="22"/>
-      <c r="AH23" s="19"/>
-      <c r="AI23" s="20"/>
-      <c r="AJ23" s="20"/>
-      <c r="AK23" s="20"/>
+      <c r="AG23" s="23"/>
+      <c r="AH23" s="20"/>
+      <c r="AI23" s="21"/>
+      <c r="AJ23" s="21"/>
+      <c r="AK23" s="21"/>
       <c r="AMJ23" s="0"/>
     </row>
     <row r="24" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="18" t="n">
+      <c r="C24" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D24" s="18" t="n">
+      <c r="D24" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="18" t="n">
+      <c r="E24" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F24" s="18" t="n">
+      <c r="F24" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="G24" s="18" t="n">
+      <c r="G24" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="H24" s="18" t="n">
+      <c r="H24" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="I24" s="18" t="n">
+      <c r="I24" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="J24" s="18" t="n">
+      <c r="J24" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="K24" s="18" t="n">
+      <c r="K24" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="L24" s="18" t="n">
+      <c r="L24" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="M24" s="18" t="n">
+      <c r="M24" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="N24" s="18" t="n">
+      <c r="N24" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="O24" s="18" t="n">
+      <c r="O24" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="P24" s="18" t="n">
+      <c r="P24" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="Q24" s="18" t="n">
+      <c r="Q24" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="R24" s="18" t="n">
+      <c r="R24" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="S24" s="18" t="n">
+      <c r="S24" s="19" t="n">
         <v>17</v>
       </c>
-      <c r="T24" s="18" t="n">
+      <c r="T24" s="19" t="n">
         <v>18</v>
       </c>
-      <c r="U24" s="18" t="n">
+      <c r="U24" s="19" t="n">
         <v>19</v>
       </c>
-      <c r="V24" s="18" t="n">
+      <c r="V24" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="W24" s="18" t="n">
+      <c r="W24" s="19" t="n">
         <v>21</v>
       </c>
-      <c r="X24" s="18" t="n">
+      <c r="X24" s="19" t="n">
         <v>22</v>
       </c>
-      <c r="Y24" s="18" t="n">
+      <c r="Y24" s="19" t="n">
         <v>23</v>
       </c>
-      <c r="Z24" s="18" t="n">
+      <c r="Z24" s="19" t="n">
         <v>24</v>
       </c>
-      <c r="AA24" s="18" t="n">
+      <c r="AA24" s="19" t="n">
         <v>25</v>
       </c>
-      <c r="AB24" s="18" t="n">
+      <c r="AB24" s="19" t="n">
         <v>26</v>
       </c>
-      <c r="AC24" s="18" t="n">
+      <c r="AC24" s="19" t="n">
         <v>27</v>
       </c>
-      <c r="AD24" s="18" t="n">
+      <c r="AD24" s="19" t="n">
         <v>28</v>
       </c>
-      <c r="AE24" s="18" t="n">
+      <c r="AE24" s="19" t="n">
         <v>29</v>
       </c>
-      <c r="AF24" s="18" t="n">
+      <c r="AF24" s="19" t="n">
         <v>30</v>
       </c>
-      <c r="AG24" s="18" t="n">
+      <c r="AG24" s="19" t="n">
         <v>31</v>
       </c>
-      <c r="AH24" s="19" t="n">
+      <c r="AH24" s="20" t="n">
         <f aca="false">COUNTIF($C25:$AG25,"T")</f>
         <v>0</v>
       </c>
-      <c r="AI24" s="20" t="n">
+      <c r="AI24" s="21" t="n">
         <f aca="false">COUNTIF($C25:$AG25,"U")</f>
         <v>0</v>
       </c>
-      <c r="AJ24" s="20" t="n">
+      <c r="AJ24" s="21" t="n">
         <f aca="false">COUNTIF($C25:$AG25,"E")</f>
         <v>0</v>
       </c>
-      <c r="AK24" s="20" t="n">
+      <c r="AK24" s="21" t="n">
         <f aca="false">COUNTIF($C25:$AG25,"P")</f>
         <v>0</v>
       </c>
       <c r="AMJ24" s="0"/>
     </row>
     <row r="25" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="17"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
-      <c r="N25" s="21"/>
-      <c r="O25" s="21"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
       <c r="P25" s="10"/>
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
       <c r="T25" s="10"/>
-      <c r="U25" s="21"/>
-      <c r="V25" s="21"/>
+      <c r="U25" s="22"/>
+      <c r="V25" s="22"/>
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
       <c r="Y25" s="10"/>
       <c r="Z25" s="10"/>
       <c r="AA25" s="10"/>
-      <c r="AB25" s="21"/>
-      <c r="AC25" s="21"/>
+      <c r="AB25" s="22"/>
+      <c r="AC25" s="22"/>
       <c r="AD25" s="10"/>
       <c r="AE25" s="10"/>
       <c r="AF25" s="10"/>
       <c r="AG25" s="10"/>
-      <c r="AH25" s="19"/>
-      <c r="AI25" s="20"/>
-      <c r="AJ25" s="20"/>
-      <c r="AK25" s="20"/>
+      <c r="AH25" s="20"/>
+      <c r="AI25" s="21"/>
+      <c r="AJ25" s="21"/>
+      <c r="AK25" s="21"/>
       <c r="AMJ25" s="0"/>
     </row>
     <row r="26" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="18" t="n">
+      <c r="C26" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="18" t="n">
+      <c r="D26" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E26" s="18" t="n">
+      <c r="E26" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F26" s="18" t="n">
+      <c r="F26" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="G26" s="18" t="n">
+      <c r="G26" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="H26" s="18" t="n">
+      <c r="H26" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="I26" s="18" t="n">
+      <c r="I26" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="J26" s="18" t="n">
+      <c r="J26" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="K26" s="18" t="n">
+      <c r="K26" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="L26" s="18" t="n">
+      <c r="L26" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="M26" s="18" t="n">
+      <c r="M26" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="N26" s="18" t="n">
+      <c r="N26" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="O26" s="18" t="n">
+      <c r="O26" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="P26" s="18" t="n">
+      <c r="P26" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="Q26" s="18" t="n">
+      <c r="Q26" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="R26" s="18" t="n">
+      <c r="R26" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="S26" s="18" t="n">
+      <c r="S26" s="19" t="n">
         <v>17</v>
       </c>
-      <c r="T26" s="18" t="n">
+      <c r="T26" s="19" t="n">
         <v>18</v>
       </c>
-      <c r="U26" s="18" t="n">
+      <c r="U26" s="19" t="n">
         <v>19</v>
       </c>
-      <c r="V26" s="18" t="n">
+      <c r="V26" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="W26" s="18" t="n">
+      <c r="W26" s="19" t="n">
         <v>21</v>
       </c>
-      <c r="X26" s="18" t="n">
+      <c r="X26" s="19" t="n">
         <v>22</v>
       </c>
-      <c r="Y26" s="18" t="n">
+      <c r="Y26" s="19" t="n">
         <v>23</v>
       </c>
-      <c r="Z26" s="18" t="n">
+      <c r="Z26" s="19" t="n">
         <v>24</v>
       </c>
-      <c r="AA26" s="18" t="n">
+      <c r="AA26" s="19" t="n">
         <v>25</v>
       </c>
-      <c r="AB26" s="18" t="n">
+      <c r="AB26" s="19" t="n">
         <v>26</v>
       </c>
-      <c r="AC26" s="18" t="n">
+      <c r="AC26" s="19" t="n">
         <v>27</v>
       </c>
-      <c r="AD26" s="18" t="n">
+      <c r="AD26" s="19" t="n">
         <v>28</v>
       </c>
-      <c r="AE26" s="18" t="n">
+      <c r="AE26" s="19" t="n">
         <v>29</v>
       </c>
-      <c r="AF26" s="18" t="n">
+      <c r="AF26" s="19" t="n">
         <v>30</v>
       </c>
-      <c r="AG26" s="18"/>
-      <c r="AH26" s="19" t="n">
+      <c r="AG26" s="19"/>
+      <c r="AH26" s="20" t="n">
         <f aca="false">COUNTIF($C27:$AF27,"T")</f>
         <v>0</v>
       </c>
-      <c r="AI26" s="20" t="n">
+      <c r="AI26" s="21" t="n">
         <f aca="false">COUNTIF($C27:$AF27,"U")</f>
         <v>0</v>
       </c>
-      <c r="AJ26" s="20" t="n">
+      <c r="AJ26" s="21" t="n">
         <f aca="false">COUNTIF($C27:$AF27,"E")</f>
         <v>0</v>
       </c>
-      <c r="AK26" s="20" t="n">
+      <c r="AK26" s="21" t="n">
         <f aca="false">COUNTIF($C27:$AF27,"P")</f>
         <v>0</v>
       </c>
       <c r="AMJ26" s="0"/>
     </row>
     <row r="27" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="17"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="10"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
-      <c r="R27" s="21"/>
-      <c r="S27" s="21"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
       <c r="T27" s="10"/>
       <c r="U27" s="10"/>
       <c r="V27" s="10"/>
       <c r="W27" s="10"/>
       <c r="X27" s="10"/>
-      <c r="Y27" s="21"/>
-      <c r="Z27" s="21"/>
+      <c r="Y27" s="22"/>
+      <c r="Z27" s="22"/>
       <c r="AA27" s="10"/>
       <c r="AB27" s="10"/>
       <c r="AC27" s="10"/>
       <c r="AD27" s="10"/>
       <c r="AE27" s="10"/>
-      <c r="AF27" s="21"/>
-      <c r="AG27" s="22"/>
-      <c r="AH27" s="19"/>
-      <c r="AI27" s="20"/>
-      <c r="AJ27" s="20"/>
-      <c r="AK27" s="20"/>
+      <c r="AF27" s="22"/>
+      <c r="AG27" s="23"/>
+      <c r="AH27" s="20"/>
+      <c r="AI27" s="21"/>
+      <c r="AJ27" s="21"/>
+      <c r="AK27" s="21"/>
       <c r="AMJ27" s="0"/>
     </row>
     <row r="28" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18" t="n">
+      <c r="C28" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D28" s="18" t="n">
+      <c r="D28" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="E28" s="18" t="n">
+      <c r="E28" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F28" s="18" t="n">
+      <c r="F28" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="G28" s="18" t="n">
+      <c r="G28" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="H28" s="18" t="n">
+      <c r="H28" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="I28" s="18" t="n">
+      <c r="I28" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="J28" s="18" t="n">
+      <c r="J28" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="K28" s="18" t="n">
+      <c r="K28" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="L28" s="18" t="n">
+      <c r="L28" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="M28" s="18" t="n">
+      <c r="M28" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="N28" s="18" t="n">
+      <c r="N28" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="O28" s="18" t="n">
+      <c r="O28" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="P28" s="18" t="n">
+      <c r="P28" s="19" t="n">
         <v>14</v>
       </c>
-      <c r="Q28" s="18" t="n">
+      <c r="Q28" s="19" t="n">
         <v>15</v>
       </c>
-      <c r="R28" s="18" t="n">
+      <c r="R28" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="S28" s="18" t="n">
+      <c r="S28" s="19" t="n">
         <v>17</v>
       </c>
-      <c r="T28" s="18" t="n">
+      <c r="T28" s="19" t="n">
         <v>18</v>
       </c>
-      <c r="U28" s="18" t="n">
+      <c r="U28" s="19" t="n">
         <v>19</v>
       </c>
-      <c r="V28" s="18" t="n">
+      <c r="V28" s="19" t="n">
         <v>20</v>
       </c>
-      <c r="W28" s="18" t="n">
+      <c r="W28" s="19" t="n">
         <v>21</v>
       </c>
-      <c r="X28" s="18" t="n">
+      <c r="X28" s="19" t="n">
         <v>22</v>
       </c>
-      <c r="Y28" s="18" t="n">
+      <c r="Y28" s="19" t="n">
         <v>23</v>
       </c>
-      <c r="Z28" s="18" t="n">
+      <c r="Z28" s="19" t="n">
         <v>24</v>
       </c>
-      <c r="AA28" s="18" t="n">
+      <c r="AA28" s="19" t="n">
         <v>25</v>
       </c>
-      <c r="AB28" s="18" t="n">
+      <c r="AB28" s="19" t="n">
         <v>26</v>
       </c>
-      <c r="AC28" s="18" t="n">
+      <c r="AC28" s="19" t="n">
         <v>27</v>
       </c>
-      <c r="AD28" s="18" t="n">
+      <c r="AD28" s="19" t="n">
         <v>28</v>
       </c>
-      <c r="AE28" s="18" t="n">
+      <c r="AE28" s="19" t="n">
         <v>29</v>
       </c>
-      <c r="AF28" s="18" t="n">
+      <c r="AF28" s="19" t="n">
         <v>30</v>
       </c>
-      <c r="AG28" s="18" t="n">
+      <c r="AG28" s="19" t="n">
         <v>31</v>
       </c>
-      <c r="AH28" s="19" t="n">
+      <c r="AH28" s="20" t="n">
         <f aca="false">COUNTIF($C29:$AG29,"T")</f>
         <v>0</v>
       </c>
-      <c r="AI28" s="20" t="n">
+      <c r="AI28" s="21" t="n">
         <f aca="false">COUNTIF($C29:$AG29,"U")</f>
         <v>0</v>
       </c>
-      <c r="AJ28" s="20" t="n">
+      <c r="AJ28" s="21" t="n">
         <f aca="false">COUNTIF($C29:$AG29,"E")</f>
         <v>0</v>
       </c>
-      <c r="AK28" s="20" t="n">
+      <c r="AK28" s="21" t="n">
         <f aca="false">COUNTIF($C29:$AG29,"P")</f>
         <v>0</v>
       </c>
       <c r="AMJ28" s="0"/>
     </row>
     <row r="29" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="17"/>
-      <c r="C29" s="21"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="22"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
-      <c r="P29" s="21"/>
-      <c r="Q29" s="21"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
       <c r="T29" s="10"/>
       <c r="U29" s="10"/>
       <c r="V29" s="10"/>
-      <c r="W29" s="21"/>
-      <c r="X29" s="21"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
       <c r="Y29" s="10"/>
       <c r="Z29" s="10"/>
       <c r="AA29" s="10"/>
       <c r="AB29" s="10"/>
       <c r="AC29" s="10"/>
-      <c r="AD29" s="21"/>
-      <c r="AE29" s="21"/>
+      <c r="AD29" s="22"/>
+      <c r="AE29" s="22"/>
       <c r="AF29" s="10"/>
       <c r="AG29" s="10"/>
-      <c r="AH29" s="19"/>
-      <c r="AI29" s="20"/>
-      <c r="AJ29" s="20"/>
-      <c r="AK29" s="20"/>
+      <c r="AH29" s="20"/>
+      <c r="AI29" s="21"/>
+      <c r="AJ29" s="21"/>
+      <c r="AK29" s="21"/>
       <c r="AMJ29" s="0"/>
     </row>
     <row r="30" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="AE30" s="24" t="s">
+      <c r="AE30" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="AF30" s="24"/>
-      <c r="AG30" s="24"/>
-      <c r="AH30" s="20" t="n">
+      <c r="AF30" s="25"/>
+      <c r="AG30" s="25"/>
+      <c r="AH30" s="26" t="n">
         <f aca="false">SUM(AH6:AH29)</f>
         <v>0</v>
       </c>
-      <c r="AI30" s="20" t="n">
+      <c r="AI30" s="26" t="n">
         <f aca="false">SUM(AI6:AI29)</f>
         <v>0</v>
       </c>
-      <c r="AJ30" s="20" t="n">
+      <c r="AJ30" s="26" t="n">
         <f aca="false">SUM(AJ6:AJ29)</f>
         <v>0</v>
       </c>
-      <c r="AK30" s="20" t="n">
+      <c r="AK30" s="26" t="n">
         <f aca="false">SUM(AK6:AK29)</f>
         <v>0</v>
       </c>

</xml_diff>